<commit_message>
Fixed outdated references to the servo thread being on core 0.
</commit_message>
<xml_diff>
--- a/Documentation/Threads.xlsx
+++ b/Documentation/Threads.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
         <v>10</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixed SPI core assignment.
</commit_message>
<xml_diff>
--- a/Documentation/Threads.xlsx
+++ b/Documentation/Threads.xlsx
@@ -411,7 +411,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Combined motor/servo PWM threads in documentation.
</commit_message>
<xml_diff>
--- a/Documentation/Threads.xlsx
+++ b/Documentation/Threads.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Thread</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Gadgeteer</t>
   </si>
   <si>
-    <t>Motor PWM</t>
-  </si>
-  <si>
-    <t>Servo PWM</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -70,6 +64,9 @@
   </si>
   <si>
     <t>User-defined (for reference):</t>
+  </si>
+  <si>
+    <t>PWM</t>
   </si>
 </sst>
 </file>
@@ -408,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A9" sqref="A9:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,18 +429,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -456,7 +453,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -480,100 +477,92 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>